<commit_message>
Update pre-processing Nias 1911 for multiple forms in lexeme and note form.
</commit_message>
<xml_diff>
--- a/C-grp-02-HolleList-01_28383_assignsubmission_file/NIAS_1911/NIAS_1911_NOTE.xlsx
+++ b/C-grp-02-HolleList-01_28383_assignsubmission_file/NIAS_1911/NIAS_1911_NOTE.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Primahadi/Documents/research/Lexiology_Lexicography_Even-2024_Holle_List_Barrier_Islands/C-grp-02-HolleList-01_28383_assignsubmission_file/NIAS_1911/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B594CFD8-CF63-4C4C-A4E4-5C9598317262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{792C8552-CBB3-B646-97A5-13D87467E74E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13980" yWindow="500" windowWidth="14820" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$167</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="268">
   <si>
     <t>ID</t>
   </si>
@@ -234,9 +237,6 @@
     <t>sifagelo, fa'elo , sifa'elo</t>
   </si>
   <si>
-    <t>(a small kind of parrot )</t>
-  </si>
-  <si>
     <t>here only the ... &lt;?&gt; ... is known</t>
   </si>
   <si>
@@ -336,15 +336,9 @@
     <t>this is a cargo &lt;?&gt;</t>
   </si>
   <si>
-    <t>aloecha, sole</t>
-  </si>
-  <si>
     <t>small, large</t>
   </si>
   <si>
-    <t xml:space="preserve">sola , manola , alachai , mangal </t>
-  </si>
-  <si>
     <t>.</t>
   </si>
   <si>
@@ -606,9 +600,6 @@
     <t>calf</t>
   </si>
   <si>
-    <t>(small)</t>
-  </si>
-  <si>
     <t>fôtô</t>
   </si>
   <si>
@@ -747,9 +738,6 @@
     <t>olifoe</t>
   </si>
   <si>
-    <t>(pronoun)</t>
-  </si>
-  <si>
     <t>ohe , mo lohe , doro , mondroro</t>
   </si>
   <si>
@@ -835,6 +823,15 @@
   </si>
   <si>
     <t>8-9 p.m.</t>
+  </si>
+  <si>
+    <t>sola , manola , alachai , mangal</t>
+  </si>
+  <si>
+    <t>aloecha, sola</t>
+  </si>
+  <si>
+    <t>(a small kind of parrot)</t>
   </si>
 </sst>
 </file>
@@ -1197,9 +1194,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F167"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="268" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A154" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D160" sqref="D160"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="268" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F133" sqref="F133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1227,7 +1224,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1306,13 +1303,13 @@
         <v>151</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C8" s="1">
         <v>7</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1320,13 +1317,13 @@
         <v>151</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C9" s="1">
         <v>7</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1345,7 +1342,7 @@
         <v>165</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="C11" s="1">
         <v>9</v>
@@ -1393,13 +1390,13 @@
         <v>182</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C15" s="1">
         <v>13</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1407,13 +1404,13 @@
         <v>182</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C16" s="1">
         <v>13</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1432,7 +1429,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C18" s="1">
         <v>15</v>
@@ -1443,7 +1440,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C19" s="1">
         <v>16</v>
@@ -1454,7 +1451,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C20" s="1">
         <v>17</v>
@@ -1466,13 +1463,13 @@
         <v>19</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C21" s="1">
         <v>17</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1480,13 +1477,13 @@
         <v>295</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C22" s="1">
         <v>18</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1494,13 +1491,13 @@
         <v>295</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C23" s="1">
         <v>18</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1508,13 +1505,13 @@
         <v>20</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C24" s="1">
         <v>19</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1522,13 +1519,13 @@
         <v>20</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C25" s="1">
         <v>19</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1558,7 +1555,7 @@
         <v>331</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C28" s="1">
         <v>22</v>
@@ -1573,7 +1570,7 @@
         <v>23</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1581,7 +1578,7 @@
         <v>340</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C30" s="1">
         <v>24</v>
@@ -1604,13 +1601,13 @@
         <v>24</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C32" s="1">
         <v>26</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1624,7 +1621,7 @@
         <v>27</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1679,13 +1676,13 @@
         <v>400</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C38" s="1">
         <v>32</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1705,13 +1702,13 @@
         <v>451</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C40" s="1">
         <v>34</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1719,13 +1716,13 @@
         <v>451</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C41" s="1">
         <v>34</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1738,7 +1735,7 @@
       </c>
       <c r="D42" s="1"/>
       <c r="F42" s="5" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1766,10 +1763,10 @@
         <v>36</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1854,7 +1851,7 @@
         <v>46</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C50" s="1">
         <v>39</v>
@@ -1901,13 +1898,13 @@
         <v>548</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C54" s="1">
         <v>43</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.15">
@@ -1919,7 +1916,7 @@
       </c>
       <c r="D55" s="1"/>
       <c r="F55" s="5" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.15">
@@ -1933,7 +1930,7 @@
         <v>51</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="28" x14ac:dyDescent="0.15">
@@ -1966,7 +1963,7 @@
         <v>604</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C59" s="1">
         <v>47</v>
@@ -2019,7 +2016,7 @@
         <v>61</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C63" s="1">
         <v>50</v>
@@ -2030,7 +2027,7 @@
         <v>61</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C64" s="1">
         <v>50</v>
@@ -2080,13 +2077,13 @@
         <v>775</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C68" s="1">
         <v>54</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="14" x14ac:dyDescent="0.15">
@@ -2094,13 +2091,13 @@
         <v>775</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C69" s="1">
         <v>54</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="14" x14ac:dyDescent="0.15">
@@ -2108,13 +2105,13 @@
         <v>775</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C70" s="1">
         <v>54</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="14" x14ac:dyDescent="0.15">
@@ -2147,7 +2144,7 @@
         <v>57</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>69</v>
+        <v>267</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="14" x14ac:dyDescent="0.15">
@@ -2155,15 +2152,15 @@
         <v>843</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C74" s="1">
         <v>58</v>
       </c>
-      <c r="D74" s="1"/>
-      <c r="F74" s="5" t="s">
-        <v>193</v>
-      </c>
+      <c r="D74" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F74" s="5"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A75" s="1">
@@ -2173,7 +2170,7 @@
         <v>59</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="14" x14ac:dyDescent="0.15">
@@ -2181,13 +2178,13 @@
         <v>861</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C76" s="1">
         <v>60</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="14" x14ac:dyDescent="0.15">
@@ -2195,13 +2192,13 @@
         <v>861</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C77" s="1">
         <v>60</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="14" x14ac:dyDescent="0.15">
@@ -2209,13 +2206,13 @@
         <v>861</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C78" s="1">
         <v>60</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="14" x14ac:dyDescent="0.15">
@@ -2223,13 +2220,13 @@
         <v>861</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C79" s="1">
         <v>60</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="14" x14ac:dyDescent="0.15">
@@ -2237,13 +2234,13 @@
         <v>861</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C80" s="1">
         <v>60</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="14" x14ac:dyDescent="0.15">
@@ -2251,13 +2248,13 @@
         <v>884</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C81" s="1">
         <v>61</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="14" x14ac:dyDescent="0.15">
@@ -2265,13 +2262,13 @@
         <v>884</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C82" s="1">
         <v>61</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="14" x14ac:dyDescent="0.15">
@@ -2279,13 +2276,13 @@
         <v>884</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C83" s="1">
         <v>61</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="14" x14ac:dyDescent="0.15">
@@ -2293,13 +2290,13 @@
         <v>884</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C84" s="1">
         <v>61</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="85" spans="1:6" ht="14" x14ac:dyDescent="0.15">
@@ -2307,13 +2304,13 @@
         <v>886</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C85" s="1">
         <v>62</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="14" x14ac:dyDescent="0.15">
@@ -2321,13 +2318,13 @@
         <v>886</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C86" s="1">
         <v>62</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="87" spans="1:6" ht="14" x14ac:dyDescent="0.15">
@@ -2335,13 +2332,13 @@
         <v>886</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C87" s="1">
         <v>62</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="14" x14ac:dyDescent="0.15">
@@ -2349,13 +2346,13 @@
         <v>886</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C88" s="1">
         <v>62</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="14" x14ac:dyDescent="0.15">
@@ -2363,13 +2360,13 @@
         <v>886</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C89" s="1">
         <v>62</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.15">
@@ -2380,7 +2377,7 @@
         <v>63</v>
       </c>
       <c r="F90" s="5" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.15">
@@ -2391,7 +2388,7 @@
         <v>64</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="14" x14ac:dyDescent="0.15">
@@ -2399,13 +2396,13 @@
         <v>912</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C92" s="1">
         <v>65</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="93" spans="1:6" ht="14" x14ac:dyDescent="0.15">
@@ -2413,13 +2410,13 @@
         <v>912</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C93" s="1">
         <v>65</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="94" spans="1:6" ht="14" x14ac:dyDescent="0.15">
@@ -2427,13 +2424,13 @@
         <v>912</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C94" s="1">
         <v>65</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="95" spans="1:6" ht="28" x14ac:dyDescent="0.15">
@@ -2441,7 +2438,7 @@
         <v>932</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C95" s="1">
         <v>66</v>
@@ -2452,7 +2449,7 @@
         <v>937</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C96" s="1">
         <v>67</v>
@@ -2467,7 +2464,7 @@
       </c>
       <c r="D97" s="1"/>
       <c r="F97" s="5" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="98" spans="1:6" ht="28" x14ac:dyDescent="0.15">
@@ -2475,7 +2472,7 @@
         <v>941</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C98" s="1">
         <v>69</v>
@@ -2486,7 +2483,7 @@
         <v>943</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C99" s="1">
         <v>70</v>
@@ -2497,7 +2494,7 @@
         <v>969</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C100" s="1">
         <v>71</v>
@@ -2505,78 +2502,78 @@
     </row>
     <row r="101" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A101" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C101" s="1">
         <v>72</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="102" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A102" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C102" s="1">
         <v>72</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="E102" s="1"/>
     </row>
     <row r="103" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A103" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C103" s="1">
         <v>72</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="E103" s="1"/>
     </row>
     <row r="104" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A104" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C104" s="1">
         <v>72</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="E104" s="1"/>
     </row>
     <row r="105" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A105" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C105" s="1">
         <v>72</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="E105" s="1"/>
     </row>
@@ -2585,16 +2582,16 @@
         <v>1028</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C106" s="1">
         <v>73</v>
       </c>
       <c r="D106" s="5" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="107" spans="1:6" ht="14" x14ac:dyDescent="0.15">
@@ -2602,16 +2599,16 @@
         <v>1028</v>
       </c>
       <c r="B107" s="6" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C107" s="1">
         <v>73</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="108" spans="1:6" ht="14" x14ac:dyDescent="0.15">
@@ -2619,16 +2616,16 @@
         <v>1028</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C108" s="1">
         <v>73</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="109" spans="1:6" ht="14" x14ac:dyDescent="0.15">
@@ -2636,28 +2633,28 @@
         <v>1028</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C109" s="1">
         <v>73</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A110" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B110" s="6"/>
       <c r="C110" s="1">
         <v>74</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.15">
@@ -2669,7 +2666,7 @@
         <v>75</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="112" spans="1:6" ht="14" x14ac:dyDescent="0.15">
@@ -2677,13 +2674,13 @@
         <v>1040</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>103</v>
+        <v>266</v>
       </c>
       <c r="C112" s="1">
         <v>76</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="113" spans="1:6" ht="28" x14ac:dyDescent="0.15">
@@ -2691,7 +2688,7 @@
         <v>1043</v>
       </c>
       <c r="B113" s="6" t="s">
-        <v>105</v>
+        <v>265</v>
       </c>
       <c r="C113" s="1">
         <v>77</v>
@@ -2702,16 +2699,16 @@
         <v>1052</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C114" s="1">
         <v>78</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="115" spans="1:6" ht="14" x14ac:dyDescent="0.15">
@@ -2719,28 +2716,28 @@
         <v>1052</v>
       </c>
       <c r="B115" s="6" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C115" s="1">
         <v>78</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E115" s="1"/>
     </row>
     <row r="116" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A116" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B116" s="6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C116" s="1">
         <v>79</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.15">
@@ -2752,7 +2749,7 @@
         <v>80</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="118" spans="1:6" ht="28" x14ac:dyDescent="0.15">
@@ -2760,7 +2757,7 @@
         <v>1127</v>
       </c>
       <c r="B118" s="6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C118" s="1">
         <v>81</v>
@@ -2768,30 +2765,30 @@
     </row>
     <row r="119" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A119" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B119" s="6" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C119" s="1">
         <v>82</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="120" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A120" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B120" s="6" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C120" s="1">
         <v>82</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="121" spans="1:6" ht="28" x14ac:dyDescent="0.15">
@@ -2799,7 +2796,7 @@
         <v>1174</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C121" s="1">
         <v>83</v>
@@ -2814,7 +2811,7 @@
         <v>84</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="123" spans="1:6" ht="14" x14ac:dyDescent="0.15">
@@ -2822,13 +2819,13 @@
         <v>1180</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C123" s="1">
         <v>85</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="124" spans="1:6" ht="14" x14ac:dyDescent="0.15">
@@ -2836,7 +2833,7 @@
         <v>1180</v>
       </c>
       <c r="B124" s="6" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C124" s="1">
         <v>85</v>
@@ -2848,7 +2845,7 @@
         <v>1193</v>
       </c>
       <c r="B125" s="6" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C125" s="1">
         <v>86</v>
@@ -2859,7 +2856,7 @@
         <v>1197</v>
       </c>
       <c r="B126" s="6" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C126" s="1">
         <v>87</v>
@@ -2867,16 +2864,14 @@
       <c r="D126" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F126" s="5" t="s">
-        <v>240</v>
-      </c>
+      <c r="F126" s="5"/>
     </row>
     <row r="127" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A127" s="1">
         <v>1206</v>
       </c>
       <c r="B127" s="6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C127" s="1">
         <v>88</v>
@@ -2884,10 +2879,10 @@
     </row>
     <row r="128" spans="1:6" ht="28" x14ac:dyDescent="0.15">
       <c r="A128" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B128" s="6" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C128" s="1">
         <v>89</v>
@@ -2898,7 +2893,7 @@
         <v>1216</v>
       </c>
       <c r="B129" s="6" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="C129" s="1">
         <v>90</v>
@@ -2909,13 +2904,13 @@
         <v>1216</v>
       </c>
       <c r="B130" s="6" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="C130" s="1">
         <v>90</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="131" spans="1:6" ht="28" x14ac:dyDescent="0.15">
@@ -2923,7 +2918,7 @@
         <v>1224</v>
       </c>
       <c r="B131" s="6" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="C131" s="1">
         <v>91</v>
@@ -2934,7 +2929,7 @@
         <v>1228</v>
       </c>
       <c r="B132" s="6" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C132" s="1">
         <v>92</v>
@@ -2942,7 +2937,7 @@
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A133" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B133" s="6"/>
       <c r="C133" s="1">
@@ -2957,7 +2952,7 @@
         <v>1145</v>
       </c>
       <c r="B134" s="6" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C134" s="1">
         <v>94</v>
@@ -2968,7 +2963,7 @@
         <v>1146</v>
       </c>
       <c r="B135" s="6" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="C135" s="1">
         <v>95</v>
@@ -2980,13 +2975,13 @@
         <v>1146</v>
       </c>
       <c r="B136" s="6" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="C136" s="1">
         <v>95</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="137" spans="1:6" ht="28" x14ac:dyDescent="0.15">
@@ -2994,7 +2989,7 @@
         <v>1151</v>
       </c>
       <c r="B137" s="6" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C137" s="1">
         <v>96</v>
@@ -3005,7 +3000,7 @@
         <v>1159</v>
       </c>
       <c r="B138" s="6" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C138" s="1">
         <v>97</v>
@@ -3013,10 +3008,10 @@
     </row>
     <row r="139" spans="1:6" ht="28" x14ac:dyDescent="0.15">
       <c r="A139" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B139" s="6" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C139" s="1">
         <v>98</v>
@@ -3027,7 +3022,7 @@
         <v>1271</v>
       </c>
       <c r="B140" s="6" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C140" s="1">
         <v>99</v>
@@ -3038,7 +3033,7 @@
         <v>1276</v>
       </c>
       <c r="B141" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C141" s="1">
         <v>100</v>
@@ -3049,7 +3044,7 @@
         <v>1284</v>
       </c>
       <c r="B142" s="6" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C142" s="1">
         <v>101</v>
@@ -3060,7 +3055,7 @@
         <v>1286</v>
       </c>
       <c r="B143" s="6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C143" s="1">
         <v>102</v>
@@ -3071,7 +3066,7 @@
         <v>1291</v>
       </c>
       <c r="B144" s="6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C144" s="1">
         <v>103</v>
@@ -3082,21 +3077,21 @@
         <v>1339</v>
       </c>
       <c r="B145" s="6" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C145" s="1">
         <v>104</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="146" spans="1:6" ht="28" x14ac:dyDescent="0.15">
       <c r="A146" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B146" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C146" s="1">
         <v>105</v>
@@ -3104,17 +3099,17 @@
     </row>
     <row r="147" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A147" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B147" s="6" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="C147" s="1">
         <v>105</v>
       </c>
       <c r="D147" s="1"/>
       <c r="F147" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.15">
@@ -3126,7 +3121,7 @@
         <v>106</v>
       </c>
       <c r="F148" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="149" spans="1:6" ht="14" x14ac:dyDescent="0.15">
@@ -3134,7 +3129,7 @@
         <v>1367</v>
       </c>
       <c r="B149" s="6" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="C149" s="1">
         <v>107</v>
@@ -3149,7 +3144,7 @@
         <v>108</v>
       </c>
       <c r="F150" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="151" spans="1:6" ht="14" x14ac:dyDescent="0.15">
@@ -3157,7 +3152,7 @@
         <v>1382</v>
       </c>
       <c r="B151" s="6" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C151" s="1">
         <v>109</v>
@@ -3168,13 +3163,13 @@
         <v>1382</v>
       </c>
       <c r="B152" s="6" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="C152" s="1">
         <v>109</v>
       </c>
       <c r="F152" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="153" spans="1:6" ht="14" x14ac:dyDescent="0.15">
@@ -3182,7 +3177,7 @@
         <v>1385</v>
       </c>
       <c r="B153" s="6" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="C153" s="1">
         <v>110</v>
@@ -3193,7 +3188,7 @@
         <v>1386</v>
       </c>
       <c r="B154" s="6" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="C154" s="1">
         <v>111</v>
@@ -3204,7 +3199,7 @@
         <v>1388</v>
       </c>
       <c r="B155" s="6" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="C155" s="1">
         <v>112</v>
@@ -3215,7 +3210,7 @@
         <v>1389</v>
       </c>
       <c r="B156" s="6" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="C156" s="1">
         <v>113</v>
@@ -3226,16 +3221,16 @@
         <v>1394</v>
       </c>
       <c r="B157" s="6" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C157" s="1">
         <v>114</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="158" spans="1:6" ht="14" x14ac:dyDescent="0.15">
@@ -3243,13 +3238,13 @@
         <v>1394</v>
       </c>
       <c r="B158" s="6" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="C158" s="1">
         <v>114</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="E158" s="1"/>
     </row>
@@ -3258,16 +3253,16 @@
         <v>1402</v>
       </c>
       <c r="B159" s="6" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="C159" s="1">
         <v>115</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="E159" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="160" spans="1:6" ht="14" x14ac:dyDescent="0.15">
@@ -3275,13 +3270,13 @@
         <v>1402</v>
       </c>
       <c r="B160" s="6" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="C160" s="1">
         <v>115</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="E160" s="1"/>
     </row>
@@ -3290,13 +3285,13 @@
         <v>1402</v>
       </c>
       <c r="B161" s="6" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="C161" s="1">
         <v>115</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="E161" s="1"/>
     </row>
@@ -3309,7 +3304,7 @@
         <v>116</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="163" spans="1:5" ht="14" x14ac:dyDescent="0.15">
@@ -3317,7 +3312,7 @@
         <v>1428</v>
       </c>
       <c r="B163" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C163" s="1">
         <v>117</v>
@@ -3328,7 +3323,7 @@
         <v>1437</v>
       </c>
       <c r="B164" s="6" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="C164" s="1">
         <v>118</v>
@@ -3339,13 +3334,13 @@
         <v>1440</v>
       </c>
       <c r="B165" s="6" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="C165" s="1">
         <v>119</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
     </row>
     <row r="166" spans="1:5" ht="14" x14ac:dyDescent="0.15">
@@ -3353,7 +3348,7 @@
         <v>1445</v>
       </c>
       <c r="B166" s="6" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C166" s="1">
         <v>120</v>
@@ -3364,7 +3359,7 @@
         <v>1481</v>
       </c>
       <c r="B167" s="6" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C167" s="1">
         <v>121</v>

</xml_diff>